<commit_message>
Change GameManager name to BoardManager, add ConsoleMode, change Army struct and more
</commit_message>
<xml_diff>
--- a/Features_Status.xlsx
+++ b/Features_Status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19140" windowHeight="8420"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19140" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>GameLogic.c</t>
   </si>
   <si>
-    <t>GameManager.c</t>
-  </si>
-  <si>
     <t>Asignee:</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Or</t>
+  </si>
+  <si>
+    <t>BoardManager.c</t>
   </si>
 </sst>
 </file>
@@ -119,7 +119,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -128,7 +128,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -194,12 +194,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,54 +505,54 @@
   <dimension ref="D4:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:7" ht="15" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D6" s="4"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D6" s="7"/>
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D7" s="4"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D7" s="7"/>
       <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
@@ -560,113 +560,113 @@
         <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D8" s="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D8" s="7"/>
       <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D9" s="7"/>
+      <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D9" s="4"/>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D10" s="4"/>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D10" s="7"/>
       <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D11" s="7"/>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D12" s="7"/>
+      <c r="E12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D11" s="4"/>
-      <c r="E11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D12" s="4"/>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D13" s="7"/>
+      <c r="E13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D13" s="4"/>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D14" s="5" t="s">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D15" s="4" t="s">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D15" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D16" s="4"/>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D16" s="7"/>
       <c r="E16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D17" s="4"/>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D17" s="7"/>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D18" s="4"/>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D18" s="7"/>
       <c r="E18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -687,7 +687,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -699,7 +699,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Chess Game logic implementation
</commit_message>
<xml_diff>
--- a/Features_Status.xlsx
+++ b/Features_Status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19140" windowHeight="8415"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19140" windowHeight="8420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>Console</t>
   </si>
@@ -42,9 +42,6 @@
     <t>GameLogic.c</t>
   </si>
   <si>
-    <t>Asignee:</t>
-  </si>
-  <si>
     <t>Unit:</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Implement console gui for drawing the board</t>
   </si>
   <si>
-    <t>ConsoleMode.c</t>
-  </si>
-  <si>
     <t>Implement a general GUI framework</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>Implement Save game to XML</t>
   </si>
   <si>
-    <t>GameFlow.c</t>
-  </si>
-  <si>
     <t>Create a generic GameFlow system (with function pointers)</t>
   </si>
   <si>
@@ -109,6 +100,43 @@
   </si>
   <si>
     <t>BoardManager.c</t>
+  </si>
+  <si>
+    <t>Left to do:</t>
+  </si>
+  <si>
+    <t>use isTie and isMatt..</t>
+  </si>
+  <si>
+    <t>GameFlow.c (Chess.c)</t>
+  </si>
+  <si>
+    <t>ConsoleMode.c (Chess.c)</t>
+  </si>
+  <si>
+    <t>Tested:</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>1) Go over the functions and make sure they are updated
+2) Add "Promotion type" to Move</t>
+  </si>
+  <si>
+    <t>1) Separate commands from parsing commands
+2) There's a function called "getScore" - there too we should use isTie and isMatt
+3) Support promotion commands for peons</t>
+  </si>
+  <si>
+    <t>Tomer / Or</t>
+  </si>
+  <si>
+    <t>Assignee:</t>
+  </si>
+  <si>
+    <t>1) Tests should be made
+2)  When are isMatt and isTie called? We should optimize that..</t>
   </si>
 </sst>
 </file>
@@ -119,7 +147,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -128,12 +156,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +183,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CC00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -186,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -198,8 +244,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -207,6 +263,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF99CC00"/>
+      <color rgb="FFCCCC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -502,174 +564,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:G18"/>
+  <dimension ref="D4:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D4" s="2"/>
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="D6" s="11"/>
+      <c r="E6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D6" s="7"/>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D8" s="11"/>
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D9" s="11"/>
+      <c r="E9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="D10" s="11"/>
+      <c r="E10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D11" s="11"/>
+      <c r="E11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D7" s="7"/>
-      <c r="E7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="G11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D8" s="7"/>
-      <c r="E8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D9" s="7"/>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D10" s="7"/>
-      <c r="E10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="I11" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D12" s="11"/>
+      <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D11" s="7"/>
-      <c r="E11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D12" s="7"/>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D13" s="11"/>
+      <c r="E13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D16" s="11"/>
+      <c r="E16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D17" s="11"/>
+      <c r="E17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D13" s="7"/>
-      <c r="E13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D16" s="7"/>
-      <c r="E16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D17" s="7"/>
-      <c r="E17" s="1" t="s">
+      <c r="H17" s="7"/>
+      <c r="I17" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D18" s="11"/>
+      <c r="E18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D18" s="7"/>
-      <c r="E18" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -687,7 +843,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -699,7 +855,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated BoardManager + fixes to types and logic
Warnings & Compilation errors should be gone
(except for IsPlayerVictor etc. Should be replaced with isTie and
isMatt..)
</commit_message>
<xml_diff>
--- a/Features_Status.xlsx
+++ b/Features_Status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Console</t>
   </si>
@@ -118,10 +118,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>1) Go over the functions and make sure they are updated
-2) Add "Promotion type" to Move</t>
   </si>
   <si>
     <t>1) Separate commands from parsing commands
@@ -137,6 +133,12 @@
   <si>
     <t>1) Tests should be made
 2)  When are isMatt and isTie called? We should optimize that..</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>All functions updated. No tests done.</t>
   </si>
 </sst>
 </file>
@@ -232,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -250,11 +252,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -566,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -588,7 +593,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>28</v>
@@ -598,7 +603,7 @@
       </c>
     </row>
     <row r="5" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="13" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -608,49 +613,51 @@
         <v>10</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="I5" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="4:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="D6" s="11"/>
-      <c r="E6" s="8" t="s">
+    <row r="6" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D6" s="13"/>
+      <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>34</v>
+      <c r="G6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="4:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="D7" s="11"/>
-      <c r="E7" s="12" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>38</v>
+      <c r="H7" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D8" s="11"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="8" t="s">
         <v>3</v>
       </c>
@@ -668,7 +675,7 @@
       </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D9" s="11"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="5" t="s">
         <v>13</v>
       </c>
@@ -684,7 +691,7 @@
       </c>
     </row>
     <row r="10" spans="4:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="D10" s="11"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="8" t="s">
         <v>4</v>
       </c>
@@ -692,17 +699,17 @@
         <v>15</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D11" s="11"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="8" t="s">
         <v>25</v>
       </c>
@@ -720,7 +727,7 @@
       </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D12" s="11"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
@@ -736,7 +743,7 @@
       </c>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D13" s="11"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="5" t="s">
         <v>17</v>
       </c>
@@ -768,7 +775,7 @@
       </c>
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="13" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -786,7 +793,7 @@
       </c>
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D16" s="11"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
@@ -800,7 +807,7 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D17" s="11"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="1" t="s">
         <v>19</v>
       </c>
@@ -814,7 +821,7 @@
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D18" s="11"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Pawn promotion, use isMatt/isTie and GameCommands
</commit_message>
<xml_diff>
--- a/Features_Status.xlsx
+++ b/Features_Status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19140" windowHeight="8420"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19140" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -158,12 +158,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,12 +185,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -234,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -249,18 +243,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,20 +561,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:9" ht="15" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -602,8 +592,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D5" s="13" t="s">
+    <row r="5" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D5" s="12" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -616,12 +606,12 @@
       <c r="H5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D6" s="13"/>
+      <c r="I5" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D6" s="12"/>
       <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
@@ -631,51 +621,51 @@
       <c r="G6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="4:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="D7" s="13"/>
-      <c r="E7" s="11" t="s">
+      <c r="I6" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="D7" s="12"/>
+      <c r="E7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D8" s="13"/>
-      <c r="E8" s="8" t="s">
+      <c r="I7" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D8" s="12"/>
+      <c r="E8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D9" s="13"/>
+      <c r="I8" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D9" s="12"/>
       <c r="E9" s="5" t="s">
         <v>13</v>
       </c>
@@ -686,48 +676,48 @@
         <v>11</v>
       </c>
       <c r="H9" s="5"/>
-      <c r="I9" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="4:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="D10" s="13"/>
-      <c r="E10" s="8" t="s">
+      <c r="I9" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="D10" s="12"/>
+      <c r="E10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D11" s="13"/>
-      <c r="E11" s="8" t="s">
+      <c r="I10" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D11" s="12"/>
+      <c r="E11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D12" s="13"/>
+      <c r="I11" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D12" s="12"/>
       <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
@@ -738,12 +728,12 @@
         <v>11</v>
       </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D13" s="13"/>
+      <c r="I12" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D13" s="12"/>
       <c r="E13" s="5" t="s">
         <v>17</v>
       </c>
@@ -754,11 +744,11 @@
         <v>11</v>
       </c>
       <c r="H13" s="5"/>
-      <c r="I13" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="I13" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D14" s="4" t="s">
         <v>23</v>
       </c>
@@ -770,12 +760,12 @@
         <v>11</v>
       </c>
       <c r="H14" s="7"/>
-      <c r="I14" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D15" s="13" t="s">
+      <c r="I14" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D15" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -788,12 +778,12 @@
         <v>26</v>
       </c>
       <c r="H15" s="7"/>
-      <c r="I15" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D16" s="13"/>
+      <c r="I15" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="12"/>
       <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
@@ -802,12 +792,12 @@
         <v>26</v>
       </c>
       <c r="H16" s="7"/>
-      <c r="I16" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D17" s="13"/>
+      <c r="I16" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D17" s="12"/>
       <c r="E17" s="1" t="s">
         <v>19</v>
       </c>
@@ -816,12 +806,12 @@
         <v>26</v>
       </c>
       <c r="H17" s="7"/>
-      <c r="I17" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D18" s="13"/>
+      <c r="I17" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D18" s="12"/>
       <c r="E18" s="1" t="s">
         <v>21</v>
       </c>
@@ -830,7 +820,7 @@
         <v>26</v>
       </c>
       <c r="H18" s="7"/>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -850,7 +840,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -862,7 +852,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Load and Save commands
</commit_message>
<xml_diff>
--- a/Features_Status.xlsx
+++ b/Features_Status.xlsx
@@ -562,7 +562,7 @@
   <dimension ref="D4:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -752,14 +752,14 @@
       <c r="D14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="8" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
GuiFW Implementation + SDL
</commit_message>
<xml_diff>
--- a/Features_Status.xlsx
+++ b/Features_Status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>Console</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Implement  window 3..</t>
-  </si>
-  <si>
-    <t>GuiMode.c</t>
   </si>
   <si>
     <t>Intermediate</t>
@@ -139,6 +136,12 @@
   </si>
   <si>
     <t>All functions updated. No tests done.</t>
+  </si>
+  <si>
+    <t>GuiFW.c</t>
+  </si>
+  <si>
+    <t>Sanity Tests</t>
   </si>
 </sst>
 </file>
@@ -163,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +209,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -234,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -256,12 +265,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,7 +582,7 @@
   <dimension ref="D4:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,6 +592,7 @@
     <col min="6" max="6" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:9" x14ac:dyDescent="0.35">
@@ -593,17 +604,17 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -614,32 +625,32 @@
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D6" s="13"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="4:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="D7" s="13"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="11" t="s">
         <v>2</v>
       </c>
@@ -647,17 +658,17 @@
         <v>7</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D8" s="13"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="8" t="s">
         <v>3</v>
       </c>
@@ -668,14 +679,14 @@
         <v>11</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D9" s="13"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="5" t="s">
         <v>13</v>
       </c>
@@ -687,11 +698,11 @@
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="4:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="D10" s="13"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="8" t="s">
         <v>4</v>
       </c>
@@ -699,71 +710,71 @@
         <v>15</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D11" s="13"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D12" s="13"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D13" s="13"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -771,67 +782,67 @@
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="9" t="s">
-        <v>33</v>
+      <c r="F15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D16" s="13"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D17" s="13"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D18" s="13"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>